<commit_message>
Atualizacao start_menu.py com animacao de fusao
</commit_message>
<xml_diff>
--- a/data/csv/Fusao.xlsx
+++ b/data/csv/Fusao.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luizb\Documents\LP\A2-Supernova\data\csv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luizb\Documents\LP\supernova_game\data\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEBA837E-889E-4A48-B511-4ACB7AEEE759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3DA0AF-77BB-47A5-9C0A-066990456875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{0EEE3841-29D7-4E79-BA1B-2D13D8D18CD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="124">
   <si>
     <t>Elemento 1</t>
   </si>
@@ -53,9 +54,6 @@
     <t>Produto</t>
   </si>
   <si>
-    <t>Energia</t>
-  </si>
-  <si>
     <t>He-3</t>
   </si>
   <si>
@@ -86,9 +84,6 @@
     <t>N-13</t>
   </si>
   <si>
-    <t>[C-13, e, ve]</t>
-  </si>
-  <si>
     <t>C-13</t>
   </si>
   <si>
@@ -104,9 +99,6 @@
     <t>[O-15, foton]</t>
   </si>
   <si>
-    <t>[N-15, e, ve]</t>
-  </si>
-  <si>
     <t>N-15</t>
   </si>
   <si>
@@ -122,9 +114,6 @@
     <t>[Be-7, foton]</t>
   </si>
   <si>
-    <t>pp-i</t>
-  </si>
-  <si>
     <t>Be-7</t>
   </si>
   <si>
@@ -140,9 +129,6 @@
     <t>[He-4, He-4]</t>
   </si>
   <si>
-    <t>pp-ii</t>
-  </si>
-  <si>
     <t>[B-8, foton]</t>
   </si>
   <si>
@@ -152,13 +138,277 @@
     <t>[Be-8, e+, ve]</t>
   </si>
   <si>
-    <t>pp=iii</t>
-  </si>
-  <si>
     <t>e+</t>
   </si>
   <si>
     <t>[foton, foton]</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>B-</t>
+  </si>
+  <si>
+    <t>B+</t>
+  </si>
+  <si>
+    <t>[n, e+, ve]</t>
+  </si>
+  <si>
+    <t>[p, e, ve_]</t>
+  </si>
+  <si>
+    <t>[C-13, e+, ve]</t>
+  </si>
+  <si>
+    <t>[N-15, e+, ve]</t>
+  </si>
+  <si>
+    <t>decaimento par</t>
+  </si>
+  <si>
+    <t>Triplo Alpha</t>
+  </si>
+  <si>
+    <t>Fusão do Carbono</t>
+  </si>
+  <si>
+    <t>[Mg-25, foton]</t>
+  </si>
+  <si>
+    <t>[Si-28, foton]</t>
+  </si>
+  <si>
+    <t>O-16</t>
+  </si>
+  <si>
+    <t>Ciclo CNO-I</t>
+  </si>
+  <si>
+    <t>Ciclo CNO-II</t>
+  </si>
+  <si>
+    <t>[F-17, foton]</t>
+  </si>
+  <si>
+    <t>Cadeia PP I</t>
+  </si>
+  <si>
+    <t>Cadeia PP II</t>
+  </si>
+  <si>
+    <t>Cadeia PP III</t>
+  </si>
+  <si>
+    <t>F-17</t>
+  </si>
+  <si>
+    <t>[O-17, e+, ve]</t>
+  </si>
+  <si>
+    <t>O-17</t>
+  </si>
+  <si>
+    <t>[N-14, He-4]</t>
+  </si>
+  <si>
+    <t>[Mg-23, n]</t>
+  </si>
+  <si>
+    <t>[Mg-24, foton]</t>
+  </si>
+  <si>
+    <t>[Na-23, H-1]</t>
+  </si>
+  <si>
+    <t>[Ne-20, He-4]</t>
+  </si>
+  <si>
+    <t>[O-16, He-4, He-4]</t>
+  </si>
+  <si>
+    <t>Fusão do Neônio</t>
+  </si>
+  <si>
+    <t>Ne-20</t>
+  </si>
+  <si>
+    <t>foton</t>
+  </si>
+  <si>
+    <t>[O-16, He-4]</t>
+  </si>
+  <si>
+    <t>[Ne-21, foton]</t>
+  </si>
+  <si>
+    <t>Ne-21</t>
+  </si>
+  <si>
+    <t>[Mg-24, n]</t>
+  </si>
+  <si>
+    <t>[Si-28, He-4]</t>
+  </si>
+  <si>
+    <t>[P-31, H-1]</t>
+  </si>
+  <si>
+    <t>[S-31, n]</t>
+  </si>
+  <si>
+    <t>[Si-30, H-1, H-1]</t>
+  </si>
+  <si>
+    <t>[S-32, foton]</t>
+  </si>
+  <si>
+    <t>[P-30, H-2]</t>
+  </si>
+  <si>
+    <t>[Mg-24, He-4, He-4]</t>
+  </si>
+  <si>
+    <t>Fusão do Oxigênio</t>
+  </si>
+  <si>
+    <t>Si-28</t>
+  </si>
+  <si>
+    <t>S-32</t>
+  </si>
+  <si>
+    <t>Ar-36</t>
+  </si>
+  <si>
+    <t>Ca-40</t>
+  </si>
+  <si>
+    <t>Ti-44</t>
+  </si>
+  <si>
+    <t>Cr-48</t>
+  </si>
+  <si>
+    <t>Fe-52</t>
+  </si>
+  <si>
+    <t>Ni-56</t>
+  </si>
+  <si>
+    <t>Co-56</t>
+  </si>
+  <si>
+    <t>[Co-56, e+, ve]</t>
+  </si>
+  <si>
+    <t>[Fe-56, e+, ve]</t>
+  </si>
+  <si>
+    <t>Queima do Silício</t>
+  </si>
+  <si>
+    <t>[Ni-56, foton]</t>
+  </si>
+  <si>
+    <t>[Fe-52, foton]</t>
+  </si>
+  <si>
+    <t>[Cr-48, foton]</t>
+  </si>
+  <si>
+    <t>[Ti-44, foton]</t>
+  </si>
+  <si>
+    <t>[Ca-40, foton]</t>
+  </si>
+  <si>
+    <t>[Ar-36, foton]</t>
+  </si>
+  <si>
+    <t>Camadas</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>He</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Ne</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>Fe</t>
+  </si>
+  <si>
+    <t>Processo</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>P-31</t>
+  </si>
+  <si>
+    <t>[Cl-35, foton]</t>
+  </si>
+  <si>
+    <t>Mg-24</t>
+  </si>
+  <si>
+    <t>Mg-25</t>
+  </si>
+  <si>
+    <t>[Si-29, foton]</t>
+  </si>
+  <si>
+    <t>Mg-26</t>
+  </si>
+  <si>
+    <t>[Al-26, foton]</t>
+  </si>
+  <si>
+    <t>Al-26</t>
+  </si>
+  <si>
+    <t>Na-22</t>
+  </si>
+  <si>
+    <t>[Mg-26, e+, ve]</t>
+  </si>
+  <si>
+    <t>[Ne-22, e-, ve]</t>
+  </si>
+  <si>
+    <t>[Na-22, He-4]</t>
+  </si>
+  <si>
+    <t>[H-3]</t>
+  </si>
+  <si>
+    <t>H-3</t>
+  </si>
+  <si>
+    <t>[He-3, e, ve_]</t>
+  </si>
+  <si>
+    <t>[C-14, H-1]</t>
+  </si>
+  <si>
+    <t>[O-18, foton]</t>
   </si>
 </sst>
 </file>
@@ -536,20 +786,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1D720B-7551-40E6-A447-F5FBB3C0D518}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="8" width="12" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="5" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -560,10 +811,10 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -571,13 +822,13 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2">
-        <v>0.42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -585,195 +836,865 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="F4" t="s">
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>32</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
       </c>
       <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>15</v>
-      </c>
-      <c r="C14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>17</v>
       </c>
       <c r="B15" t="s">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="D16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>20</v>
-      </c>
-      <c r="C17" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>23</v>
       </c>
       <c r="B18" t="s">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="D18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="D19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" t="s">
+        <v>70</v>
+      </c>
+      <c r="D31" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" t="s">
+        <v>73</v>
+      </c>
+      <c r="D34" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" t="s">
+        <v>74</v>
+      </c>
+      <c r="D35" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" t="s">
+        <v>77</v>
+      </c>
+      <c r="D38" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>79</v>
+      </c>
+      <c r="B39" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" t="s">
+        <v>91</v>
+      </c>
+      <c r="D39" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>79</v>
+      </c>
+      <c r="B40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" t="s">
+        <v>75</v>
+      </c>
+      <c r="D40" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" t="s">
+        <v>96</v>
+      </c>
+      <c r="D41" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>81</v>
+      </c>
+      <c r="B42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" t="s">
+        <v>95</v>
+      </c>
+      <c r="D42" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>82</v>
+      </c>
+      <c r="B43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" t="s">
+        <v>94</v>
+      </c>
+      <c r="D43" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>83</v>
+      </c>
+      <c r="B44" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" t="s">
+        <v>93</v>
+      </c>
+      <c r="D44" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>84</v>
+      </c>
+      <c r="B45" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" t="s">
+        <v>92</v>
+      </c>
+      <c r="D45" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>85</v>
+      </c>
+      <c r="B46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" t="s">
+        <v>91</v>
+      </c>
+      <c r="D46" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>86</v>
+      </c>
+      <c r="C47" t="s">
+        <v>88</v>
+      </c>
+      <c r="D47" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>87</v>
+      </c>
+      <c r="C48" t="s">
+        <v>89</v>
+      </c>
+      <c r="D48" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>3</v>
+      </c>
+      <c r="B49" t="s">
+        <v>36</v>
+      </c>
+      <c r="C49" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>120</v>
+      </c>
+      <c r="C50" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>10</v>
+      </c>
+      <c r="B51" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52" t="s">
+        <v>17</v>
+      </c>
+      <c r="C52" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>10</v>
+      </c>
+      <c r="B53" t="s">
+        <v>48</v>
+      </c>
+      <c r="C53" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>107</v>
+      </c>
+      <c r="B54" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>109</v>
+      </c>
+      <c r="B55" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>110</v>
+      </c>
+      <c r="B57" t="s">
+        <v>2</v>
+      </c>
+      <c r="C57" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>114</v>
+      </c>
+      <c r="C58" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>112</v>
+      </c>
+      <c r="B59" t="s">
+        <v>36</v>
+      </c>
+      <c r="C59" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>115</v>
+      </c>
+      <c r="C60" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>17</v>
+      </c>
+      <c r="B61" t="s">
+        <v>36</v>
+      </c>
+      <c r="C61" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>17</v>
+      </c>
+      <c r="B62" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>26</v>
+      </c>
+      <c r="B65" t="s">
+        <v>33</v>
+      </c>
+      <c r="C65" t="s">
+        <v>34</v>
+      </c>
+      <c r="D65" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>35</v>
+      </c>
+      <c r="C66" t="s">
         <v>39</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D66" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>36</v>
+      </c>
+      <c r="C67" t="s">
         <v>40</v>
+      </c>
+      <c r="D67" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6433F21A-FBF6-40D8-A1D6-6F9EACBC596B}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Criacao da tabela periodica
</commit_message>
<xml_diff>
--- a/data/csv/Fusao.xlsx
+++ b/data/csv/Fusao.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luizb\Documents\LP\supernova_game\data\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3DA0AF-77BB-47A5-9C0A-066990456875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB970F1-B3D3-433F-BF7D-B17D1655DA28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{0EEE3841-29D7-4E79-BA1B-2D13D8D18CD6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0EEE3841-29D7-4E79-BA1B-2D13D8D18CD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -788,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1D720B-7551-40E6-A447-F5FBB3C0D518}">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48:XFD48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
atualizei o video de finalização e os testes
</commit_message>
<xml_diff>
--- a/data/csv/Fusao.xlsx
+++ b/data/csv/Fusao.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luizb\Documents\LP\elemental_fusion_game\data\csv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elisa\Desktop\FGV\LP\elemental_fusion_game\data\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBFABC0F-23C3-4E98-BDB9-C5DDB4D13DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C3F25C6-123E-4C51-8ED0-4087D3F8CD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0EEE3841-29D7-4E79-BA1B-2D13D8D18CD6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0EEE3841-29D7-4E79-BA1B-2D13D8D18CD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="125">
   <si>
     <t>H-1</t>
   </si>
@@ -385,13 +385,40 @@
   </si>
   <si>
     <t>A formação do Hélio-4 marca o fim da Cadeia Proton-Proton</t>
+  </si>
+  <si>
+    <t>O Hélio-3 é um isótopo leve do hélio essencial em reações nucleares como a Cadeia Próton-Próton.</t>
+  </si>
+  <si>
+    <t>O Berílio-7 é um isótopo radioativo formado na Cadeia Próton-Próton.</t>
+  </si>
+  <si>
+    <t>O Lítio-7 é um isótopo estável formado na nucleossíntese estelar.</t>
+  </si>
+  <si>
+    <t>O Hélio-4 é um núcleo estável formado pela fusão de prótons e nêutrons.</t>
+  </si>
+  <si>
+    <t>O Boro-8 é um isótopo radioativo produzido em reações nucleares estelares.</t>
+  </si>
+  <si>
+    <t>O Berílio-8 é um isótopo extremamente instável formado em reações nucleares estelares.</t>
+  </si>
+  <si>
+    <t>O Carbono-12 é um isótopo estável formado no ciclo triple-alfa em estrelas e fundamental para a formação da vida.</t>
+  </si>
+  <si>
+    <t>O Carbono-13 é um isótopo estável do carbono que surge do decaimento do Nitrogênio-13.</t>
+  </si>
+  <si>
+    <t>O Nitrogênio-13 é um isótopo radioativo do nitrogênio.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -401,14 +428,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -436,7 +455,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -774,18 +793,18 @@
   <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
     <col min="5" max="5" width="59" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -802,7 +821,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -819,7 +838,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -832,8 +851,11 @@
       <c r="D3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -850,7 +872,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -863,8 +885,11 @@
       <c r="D5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -877,9 +902,11 @@
       <c r="D6" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E6" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -892,8 +919,11 @@
       <c r="D7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E7" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -906,8 +936,11 @@
       <c r="D8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E8" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -917,8 +950,11 @@
       <c r="D9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E9" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -931,8 +967,11 @@
       <c r="D10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E10" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -945,8 +984,11 @@
       <c r="D11" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E11" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -959,8 +1001,11 @@
       <c r="D12" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E12" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -970,8 +1015,11 @@
       <c r="D13" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E13" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -985,7 +1033,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -999,7 +1047,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -1010,7 +1058,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -1024,7 +1072,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1038,7 +1086,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1052,7 +1100,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1063,7 +1111,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1077,7 +1125,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -1091,7 +1139,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -1105,7 +1153,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -1119,7 +1167,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -1133,7 +1181,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -1147,7 +1195,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1161,7 +1209,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1175,7 +1223,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1189,7 +1237,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1203,7 +1251,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>18</v>
       </c>
@@ -1217,7 +1265,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -1231,7 +1279,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>18</v>
       </c>
@@ -1245,7 +1293,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>18</v>
       </c>
@@ -1259,7 +1307,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>18</v>
       </c>
@@ -1273,7 +1321,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>18</v>
       </c>
@@ -1287,7 +1335,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>18</v>
       </c>
@@ -1301,7 +1349,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>31</v>
       </c>
@@ -1315,7 +1363,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>31</v>
       </c>
@@ -1329,7 +1377,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>32</v>
       </c>
@@ -1343,7 +1391,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>33</v>
       </c>
@@ -1357,7 +1405,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>34</v>
       </c>
@@ -1371,7 +1419,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>35</v>
       </c>
@@ -1385,7 +1433,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>36</v>
       </c>
@@ -1399,7 +1447,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>37</v>
       </c>
@@ -1413,7 +1461,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>38</v>
       </c>
@@ -1424,7 +1472,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>39</v>
       </c>
@@ -1435,7 +1483,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>1</v>
       </c>
@@ -1446,7 +1494,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>55</v>
       </c>
@@ -1454,7 +1502,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>5</v>
       </c>
@@ -1465,7 +1513,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>5</v>
       </c>
@@ -1476,7 +1524,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>5</v>
       </c>
@@ -1487,7 +1535,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>49</v>
       </c>
@@ -1498,7 +1546,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>50</v>
       </c>
@@ -1509,7 +1557,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>51</v>
       </c>
@@ -1520,7 +1568,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>51</v>
       </c>
@@ -1531,7 +1579,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>53</v>
       </c>
@@ -1539,7 +1587,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>52</v>
       </c>
@@ -1550,7 +1598,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>54</v>
       </c>
@@ -1558,7 +1606,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>8</v>
       </c>
@@ -1569,7 +1617,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>8</v>
       </c>
@@ -1594,44 +1642,44 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
adicionei mais algumas fusões
</commit_message>
<xml_diff>
--- a/data/csv/Fusao.xlsx
+++ b/data/csv/Fusao.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elisa\Desktop\FGV\LP\elemental_fusion_game\data\csv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raphy\elemental_fusion_game\data\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C3F25C6-123E-4C51-8ED0-4087D3F8CD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB9B0335-E0EE-4DB6-9A14-62E1C9776BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0EEE3841-29D7-4E79-BA1B-2D13D8D18CD6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0EEE3841-29D7-4E79-BA1B-2D13D8D18CD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="530">
   <si>
     <t>H-1</t>
   </si>
@@ -412,6 +412,1221 @@
   </si>
   <si>
     <t>O Nitrogênio-13 é um isótopo radioativo do nitrogênio.</t>
+  </si>
+  <si>
+    <t>B-4</t>
+  </si>
+  <si>
+    <t>B-11, n, γ</t>
+  </si>
+  <si>
+    <t>Formação de Elementos Pesados</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com B-4 gera B-11, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>B-11</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>B-11, γ</t>
+  </si>
+  <si>
+    <t>Decaimento Radioativo</t>
+  </si>
+  <si>
+    <t>A reação de B-11 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Ti-4</t>
+  </si>
+  <si>
+    <t>Ti-46, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Ti-4 gera Ti-46, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Ti-46</t>
+  </si>
+  <si>
+    <t>Ti-46, γ</t>
+  </si>
+  <si>
+    <t>A reação de Ti-46 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Ca-4</t>
+  </si>
+  <si>
+    <t>Ca-48, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Ca-4 gera Ca-48, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Ca-48</t>
+  </si>
+  <si>
+    <t>Ca-48, γ</t>
+  </si>
+  <si>
+    <t>A reação de Ca-48 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Sc-4</t>
+  </si>
+  <si>
+    <t>Sc-45, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Sc-4 gera Sc-45, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Sc-45</t>
+  </si>
+  <si>
+    <t>Sc-45, γ</t>
+  </si>
+  <si>
+    <t>A reação de Sc-45 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Ni-4</t>
+  </si>
+  <si>
+    <t>Ni-58, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Ni-4 gera Ni-58, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Ni-58</t>
+  </si>
+  <si>
+    <t>Ni-58, γ</t>
+  </si>
+  <si>
+    <t>A reação de Ni-58 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Ni-64, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Ni-4 gera Ni-64, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Ni-64</t>
+  </si>
+  <si>
+    <t>Ni-64, γ</t>
+  </si>
+  <si>
+    <t>A reação de Ni-64 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>K-4</t>
+  </si>
+  <si>
+    <t>K-40, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com K-4 gera K-40, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>K-40</t>
+  </si>
+  <si>
+    <t>K-40, γ</t>
+  </si>
+  <si>
+    <t>A reação de K-40 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Br-4</t>
+  </si>
+  <si>
+    <t>Br-79, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Br-4 gera Br-79, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Br-79</t>
+  </si>
+  <si>
+    <t>Br-79, γ</t>
+  </si>
+  <si>
+    <t>A reação de Br-79 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Be-9, γ</t>
+  </si>
+  <si>
+    <t>Formação de Berílio</t>
+  </si>
+  <si>
+    <t>A fusão de dois núcleos de He-4 gera Be-9 e raios gama.</t>
+  </si>
+  <si>
+    <t>Be-9</t>
+  </si>
+  <si>
+    <t>A reação de Be-9 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Th-4</t>
+  </si>
+  <si>
+    <t>Th-232, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Th-4 gera Th-232, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Th-232</t>
+  </si>
+  <si>
+    <t>Th-232, γ</t>
+  </si>
+  <si>
+    <t>A reação de Th-232 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Ga-4</t>
+  </si>
+  <si>
+    <t>Ga-69, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Ga-4 gera Ga-69, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Ga-69</t>
+  </si>
+  <si>
+    <t>Ga-69, γ</t>
+  </si>
+  <si>
+    <t>A reação de Ga-69 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Ge-4</t>
+  </si>
+  <si>
+    <t>Ge-74, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Ge-4 gera Ge-74, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Ge-74</t>
+  </si>
+  <si>
+    <t>Ge-74, γ</t>
+  </si>
+  <si>
+    <t>A reação de Ge-74 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Ti-49, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Ti-4 gera Ti-49, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Ti-49</t>
+  </si>
+  <si>
+    <t>Ti-49, γ</t>
+  </si>
+  <si>
+    <t>A reação de Ti-49 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Kr-4</t>
+  </si>
+  <si>
+    <t>Kr-78, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Kr-4 gera Kr-78, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Kr-78</t>
+  </si>
+  <si>
+    <t>Kr-78, γ</t>
+  </si>
+  <si>
+    <t>A reação de Kr-78 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Mn-4</t>
+  </si>
+  <si>
+    <t>Mn-55, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Mn-4 gera Mn-55, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Mn-55</t>
+  </si>
+  <si>
+    <t>Mn-55, γ</t>
+  </si>
+  <si>
+    <t>A reação de Mn-55 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>F-4</t>
+  </si>
+  <si>
+    <t>F-19, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com F-4 gera F-19, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>F-19</t>
+  </si>
+  <si>
+    <t>F-19, γ</t>
+  </si>
+  <si>
+    <t>A reação de F-19 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Zn-4</t>
+  </si>
+  <si>
+    <t>Zn-66, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Zn-4 gera Zn-66, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Zn-66</t>
+  </si>
+  <si>
+    <t>Zn-66, γ</t>
+  </si>
+  <si>
+    <t>A reação de Zn-66 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Cr-4</t>
+  </si>
+  <si>
+    <t>Cr-52, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Cr-4 gera Cr-52, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Cr-52</t>
+  </si>
+  <si>
+    <t>Cr-52, γ</t>
+  </si>
+  <si>
+    <t>A reação de Cr-52 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Li-6, γ</t>
+  </si>
+  <si>
+    <t>Formação de Lítio</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com H-3 gera Li-6, liberando raios gama.</t>
+  </si>
+  <si>
+    <t>Li-6</t>
+  </si>
+  <si>
+    <t>A reação de Li-6 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Ti-48, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Ti-4 gera Ti-48, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Ti-48</t>
+  </si>
+  <si>
+    <t>Ti-48, γ</t>
+  </si>
+  <si>
+    <t>A reação de Ti-48 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Ar-4</t>
+  </si>
+  <si>
+    <t>Ar-40, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Ar-4 gera Ar-40, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Ar-40</t>
+  </si>
+  <si>
+    <t>Ar-40, γ</t>
+  </si>
+  <si>
+    <t>A reação de Ar-40 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Se-4</t>
+  </si>
+  <si>
+    <t>Se-76, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Se-4 gera Se-76, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Se-76</t>
+  </si>
+  <si>
+    <t>Se-76, γ</t>
+  </si>
+  <si>
+    <t>A reação de Se-76 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Zn-64, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Zn-4 gera Zn-64, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Zn-64</t>
+  </si>
+  <si>
+    <t>Zn-64, γ</t>
+  </si>
+  <si>
+    <t>A reação de Zn-64 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Cl-4</t>
+  </si>
+  <si>
+    <t>Cl-37, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Cl-4 gera Cl-37, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Cl-37</t>
+  </si>
+  <si>
+    <t>Cl-37, γ</t>
+  </si>
+  <si>
+    <t>A reação de Cl-37 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Ni-61, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Ni-4 gera Ni-61, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Ni-61</t>
+  </si>
+  <si>
+    <t>Ni-61, γ</t>
+  </si>
+  <si>
+    <t>A reação de Ni-61 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Ge-70, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Ge-4 gera Ge-70, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Ge-70</t>
+  </si>
+  <si>
+    <t>Ge-70, γ</t>
+  </si>
+  <si>
+    <t>A reação de Ge-70 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Zn-67, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Zn-4 gera Zn-67, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Zn-67</t>
+  </si>
+  <si>
+    <t>Zn-67, γ</t>
+  </si>
+  <si>
+    <t>A reação de Zn-67 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>V-4</t>
+  </si>
+  <si>
+    <t>V-50, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com V-4 gera V-50, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>V-50</t>
+  </si>
+  <si>
+    <t>V-50, γ</t>
+  </si>
+  <si>
+    <t>A reação de V-50 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>As-4</t>
+  </si>
+  <si>
+    <t>As-75, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com As-4 gera As-75, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>As-75</t>
+  </si>
+  <si>
+    <t>As-75, γ</t>
+  </si>
+  <si>
+    <t>A reação de As-75 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Se-78, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Se-4 gera Se-78, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Se-78</t>
+  </si>
+  <si>
+    <t>Se-78, γ</t>
+  </si>
+  <si>
+    <t>A reação de Se-78 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Kr-80, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Kr-4 gera Kr-80, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Kr-80</t>
+  </si>
+  <si>
+    <t>Kr-80, γ</t>
+  </si>
+  <si>
+    <t>A reação de Kr-80 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>U-4</t>
+  </si>
+  <si>
+    <t>U-238, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com U-4 gera U-238, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>U-238</t>
+  </si>
+  <si>
+    <t>U-238, γ</t>
+  </si>
+  <si>
+    <t>A reação de U-238 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Fe-4</t>
+  </si>
+  <si>
+    <t>Fe-57, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Fe-4 gera Fe-57, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Fe-57</t>
+  </si>
+  <si>
+    <t>Fe-57, γ</t>
+  </si>
+  <si>
+    <t>A reação de Fe-57 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>K-41, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com K-4 gera K-41, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>K-41</t>
+  </si>
+  <si>
+    <t>K-41, γ</t>
+  </si>
+  <si>
+    <t>A reação de K-41 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Kr-86, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Kr-4 gera Kr-86, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Kr-86</t>
+  </si>
+  <si>
+    <t>Kr-86, γ</t>
+  </si>
+  <si>
+    <t>A reação de Kr-86 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Cr-50, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Cr-4 gera Cr-50, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Cr-50</t>
+  </si>
+  <si>
+    <t>Cr-50, γ</t>
+  </si>
+  <si>
+    <t>A reação de Cr-50 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Zn-68, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Zn-4 gera Zn-68, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Zn-68</t>
+  </si>
+  <si>
+    <t>Zn-68, γ</t>
+  </si>
+  <si>
+    <t>A reação de Zn-68 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Ni-62, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Ni-4 gera Ni-62, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Ni-62</t>
+  </si>
+  <si>
+    <t>Ni-62, γ</t>
+  </si>
+  <si>
+    <t>A reação de Ni-62 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Ge-72, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Ge-4 gera Ge-72, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Ge-72</t>
+  </si>
+  <si>
+    <t>Ge-72, γ</t>
+  </si>
+  <si>
+    <t>A reação de Ge-72 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Cu-4</t>
+  </si>
+  <si>
+    <t>Cu-63, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Cu-4 gera Cu-63, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Cu-63</t>
+  </si>
+  <si>
+    <t>Cu-63, γ</t>
+  </si>
+  <si>
+    <t>A reação de Cu-63 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Cr-54, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Cr-4 gera Cr-54, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Cr-54</t>
+  </si>
+  <si>
+    <t>Cr-54, γ</t>
+  </si>
+  <si>
+    <t>A reação de Cr-54 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>S-4</t>
+  </si>
+  <si>
+    <t>S-34, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com S-4 gera S-34, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>S-34</t>
+  </si>
+  <si>
+    <t>S-34, γ</t>
+  </si>
+  <si>
+    <t>A reação de S-34 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Ge-73, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Ge-4 gera Ge-73, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Ge-73</t>
+  </si>
+  <si>
+    <t>Ge-73, γ</t>
+  </si>
+  <si>
+    <t>A reação de Ge-73 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>S-36, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com S-4 gera S-36, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>S-36</t>
+  </si>
+  <si>
+    <t>S-36, γ</t>
+  </si>
+  <si>
+    <t>A reação de S-36 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Ar-38, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Ar-4 gera Ar-38, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Ar-38</t>
+  </si>
+  <si>
+    <t>Ar-38, γ</t>
+  </si>
+  <si>
+    <t>A reação de Ar-38 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Ca-46, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Ca-4 gera Ca-46, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Ca-46</t>
+  </si>
+  <si>
+    <t>Ca-46, γ</t>
+  </si>
+  <si>
+    <t>A reação de Ca-46 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>S-33, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com S-4 gera S-33, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>S-33</t>
+  </si>
+  <si>
+    <t>S-33, γ</t>
+  </si>
+  <si>
+    <t>A reação de S-33 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Ca-43, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Ca-4 gera Ca-43, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Ca-43</t>
+  </si>
+  <si>
+    <t>Ca-43, γ</t>
+  </si>
+  <si>
+    <t>A reação de Ca-43 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Ni-60, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Ni-4 gera Ni-60, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Ni-60</t>
+  </si>
+  <si>
+    <t>Ni-60, γ</t>
+  </si>
+  <si>
+    <t>A reação de Ni-60 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Pu-4</t>
+  </si>
+  <si>
+    <t>Pu-239, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Pu-4 gera Pu-239, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Pu-239</t>
+  </si>
+  <si>
+    <t>Pu-239, γ</t>
+  </si>
+  <si>
+    <t>A reação de Pu-239 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Kr-83, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Kr-4 gera Kr-83, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Kr-83</t>
+  </si>
+  <si>
+    <t>Kr-83, γ</t>
+  </si>
+  <si>
+    <t>A reação de Kr-83 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Ca-44, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Ca-4 gera Ca-44, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Ca-44</t>
+  </si>
+  <si>
+    <t>Ca-44, γ</t>
+  </si>
+  <si>
+    <t>A reação de Ca-44 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Ga-71, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Ga-4 gera Ga-71, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Ga-71</t>
+  </si>
+  <si>
+    <t>Ga-71, γ</t>
+  </si>
+  <si>
+    <t>A reação de Ga-71 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>V-51, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com V-4 gera V-51, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>V-51</t>
+  </si>
+  <si>
+    <t>V-51, γ</t>
+  </si>
+  <si>
+    <t>A reação de V-51 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>K-39, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com K-4 gera K-39, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>K-39</t>
+  </si>
+  <si>
+    <t>K-39, γ</t>
+  </si>
+  <si>
+    <t>A reação de K-39 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Kr-82, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Kr-4 gera Kr-82, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Kr-82</t>
+  </si>
+  <si>
+    <t>Kr-82, γ</t>
+  </si>
+  <si>
+    <t>A reação de Kr-82 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Fe-54, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Fe-4 gera Fe-54, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Fe-54</t>
+  </si>
+  <si>
+    <t>Fe-54, γ</t>
+  </si>
+  <si>
+    <t>A reação de Fe-54 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Ti-50, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Ti-4 gera Ti-50, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Ti-50</t>
+  </si>
+  <si>
+    <t>Ti-50, γ</t>
+  </si>
+  <si>
+    <t>A reação de Ti-50 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>B-10, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com B-4 gera B-10, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>B-10</t>
+  </si>
+  <si>
+    <t>B-10, γ</t>
+  </si>
+  <si>
+    <t>A reação de B-10 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>U-235, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com U-4 gera U-235, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>U-235</t>
+  </si>
+  <si>
+    <t>U-235, γ</t>
+  </si>
+  <si>
+    <t>A reação de U-235 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Ca-42, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Ca-4 gera Ca-42, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Ca-42</t>
+  </si>
+  <si>
+    <t>Ca-42, γ</t>
+  </si>
+  <si>
+    <t>A reação de Ca-42 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Cr-53, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Cr-4 gera Cr-53, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Cr-53</t>
+  </si>
+  <si>
+    <t>Cr-53, γ</t>
+  </si>
+  <si>
+    <t>A reação de Cr-53 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Al-4</t>
+  </si>
+  <si>
+    <t>Al-27, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Al-4 gera Al-27, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Al-27</t>
+  </si>
+  <si>
+    <t>Al-27, γ</t>
+  </si>
+  <si>
+    <t>A reação de Al-27 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Co-4</t>
+  </si>
+  <si>
+    <t>Co-59, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Co-4 gera Co-59, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Co-59</t>
+  </si>
+  <si>
+    <t>Co-59, γ</t>
+  </si>
+  <si>
+    <t>A reação de Co-59 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Se-82, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Se-4 gera Se-82, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Se-82</t>
+  </si>
+  <si>
+    <t>Se-82, γ</t>
+  </si>
+  <si>
+    <t>A reação de Se-82 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Cu-65, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Cu-4 gera Cu-65, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Cu-65</t>
+  </si>
+  <si>
+    <t>Cu-65, γ</t>
+  </si>
+  <si>
+    <t>A reação de Cu-65 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Br-81, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Br-4 gera Br-81, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Br-81</t>
+  </si>
+  <si>
+    <t>Br-81, γ</t>
+  </si>
+  <si>
+    <t>A reação de Br-81 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Ti-47, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Ti-4 gera Ti-47, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Ti-47</t>
+  </si>
+  <si>
+    <t>Ti-47, γ</t>
+  </si>
+  <si>
+    <t>A reação de Ti-47 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Ge-76, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Ge-4 gera Ge-76, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Ge-76</t>
+  </si>
+  <si>
+    <t>Ge-76, γ</t>
+  </si>
+  <si>
+    <t>A reação de Ge-76 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Se-74, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Se-4 gera Se-74, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Se-74</t>
+  </si>
+  <si>
+    <t>Se-74, γ</t>
+  </si>
+  <si>
+    <t>A reação de Se-74 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Se-80, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Se-4 gera Se-80, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Se-80</t>
+  </si>
+  <si>
+    <t>Se-80, γ</t>
+  </si>
+  <si>
+    <t>A reação de Se-80 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Fe-58, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Fe-4 gera Fe-58, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Fe-58</t>
+  </si>
+  <si>
+    <t>Fe-58, γ</t>
+  </si>
+  <si>
+    <t>A reação de Fe-58 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Se-77, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Se-4 gera Se-77, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Se-77</t>
+  </si>
+  <si>
+    <t>Se-77, γ</t>
+  </si>
+  <si>
+    <t>A reação de Se-77 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Zn-70, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Zn-4 gera Zn-70, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Zn-70</t>
+  </si>
+  <si>
+    <t>Zn-70, γ</t>
+  </si>
+  <si>
+    <t>A reação de Zn-70 com emissão de raios gama.</t>
+  </si>
+  <si>
+    <t>Kr-84, n, γ</t>
+  </si>
+  <si>
+    <t>A fusão de He-4 com Kr-4 gera Kr-84, emitindo nêutrons e raios gama.</t>
+  </si>
+  <si>
+    <t>Kr-84</t>
+  </si>
+  <si>
+    <t>Kr-84, γ</t>
+  </si>
+  <si>
+    <t>A reação de Kr-84 com emissão de raios gama.</t>
   </si>
 </sst>
 </file>
@@ -453,9 +1668,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -790,21 +2004,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1D720B-7551-40E6-A447-F5FBB3C0D518}">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E211"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A62" sqref="A62:E211"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
     <col min="5" max="5" width="59" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -821,7 +2035,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -838,7 +2052,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -855,7 +2069,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -872,7 +2086,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -889,7 +2103,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -902,11 +2116,11 @@
       <c r="D6" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -919,11 +2133,11 @@
       <c r="D7" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -936,11 +2150,11 @@
       <c r="D8" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -950,11 +2164,11 @@
       <c r="D9" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -967,11 +2181,11 @@
       <c r="D10" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -984,11 +2198,11 @@
       <c r="D11" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -1001,11 +2215,11 @@
       <c r="D12" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1015,11 +2229,11 @@
       <c r="D13" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1033,7 +2247,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -1047,7 +2261,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -1058,7 +2272,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -1072,7 +2286,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1086,7 +2300,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1100,7 +2314,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1111,7 +2325,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1125,7 +2339,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -1139,7 +2353,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -1153,7 +2367,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -1167,7 +2381,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -1181,7 +2395,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -1195,7 +2409,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1209,7 +2423,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1223,7 +2437,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1237,7 +2451,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1251,7 +2465,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>18</v>
       </c>
@@ -1265,7 +2479,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -1279,7 +2493,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>18</v>
       </c>
@@ -1293,7 +2507,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>18</v>
       </c>
@@ -1307,7 +2521,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>18</v>
       </c>
@@ -1321,7 +2535,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>18</v>
       </c>
@@ -1335,7 +2549,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>18</v>
       </c>
@@ -1349,7 +2563,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>31</v>
       </c>
@@ -1363,7 +2577,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>31</v>
       </c>
@@ -1377,7 +2591,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>32</v>
       </c>
@@ -1391,7 +2605,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>33</v>
       </c>
@@ -1405,7 +2619,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>34</v>
       </c>
@@ -1419,7 +2633,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>35</v>
       </c>
@@ -1433,7 +2647,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>36</v>
       </c>
@@ -1447,7 +2661,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>37</v>
       </c>
@@ -1461,7 +2675,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>38</v>
       </c>
@@ -1472,7 +2686,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>39</v>
       </c>
@@ -1483,7 +2697,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>1</v>
       </c>
@@ -1494,7 +2708,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>55</v>
       </c>
@@ -1502,7 +2716,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>5</v>
       </c>
@@ -1513,7 +2727,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>5</v>
       </c>
@@ -1524,7 +2738,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>5</v>
       </c>
@@ -1535,7 +2749,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>49</v>
       </c>
@@ -1546,7 +2760,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>50</v>
       </c>
@@ -1557,7 +2771,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>51</v>
       </c>
@@ -1568,7 +2782,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>51</v>
       </c>
@@ -1579,7 +2793,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>53</v>
       </c>
@@ -1587,7 +2801,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>52</v>
       </c>
@@ -1598,7 +2812,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>54</v>
       </c>
@@ -1606,7 +2820,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>8</v>
       </c>
@@ -1617,7 +2831,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>8</v>
       </c>
@@ -1626,6 +2840,2556 @@
       </c>
       <c r="C61" t="s">
         <v>91</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>3</v>
+      </c>
+      <c r="B62" t="s">
+        <v>125</v>
+      </c>
+      <c r="C62" t="s">
+        <v>126</v>
+      </c>
+      <c r="D62" t="s">
+        <v>127</v>
+      </c>
+      <c r="E62" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>129</v>
+      </c>
+      <c r="B63" t="s">
+        <v>130</v>
+      </c>
+      <c r="C63" t="s">
+        <v>131</v>
+      </c>
+      <c r="D63" t="s">
+        <v>132</v>
+      </c>
+      <c r="E63" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>3</v>
+      </c>
+      <c r="B64" t="s">
+        <v>134</v>
+      </c>
+      <c r="C64" t="s">
+        <v>135</v>
+      </c>
+      <c r="D64" t="s">
+        <v>127</v>
+      </c>
+      <c r="E64" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>137</v>
+      </c>
+      <c r="B65" t="s">
+        <v>130</v>
+      </c>
+      <c r="C65" t="s">
+        <v>138</v>
+      </c>
+      <c r="D65" t="s">
+        <v>132</v>
+      </c>
+      <c r="E65" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66" t="s">
+        <v>140</v>
+      </c>
+      <c r="C66" t="s">
+        <v>141</v>
+      </c>
+      <c r="D66" t="s">
+        <v>127</v>
+      </c>
+      <c r="E66" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>143</v>
+      </c>
+      <c r="B67" t="s">
+        <v>130</v>
+      </c>
+      <c r="C67" t="s">
+        <v>144</v>
+      </c>
+      <c r="D67" t="s">
+        <v>132</v>
+      </c>
+      <c r="E67" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>3</v>
+      </c>
+      <c r="B68" t="s">
+        <v>146</v>
+      </c>
+      <c r="C68" t="s">
+        <v>147</v>
+      </c>
+      <c r="D68" t="s">
+        <v>127</v>
+      </c>
+      <c r="E68" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>149</v>
+      </c>
+      <c r="B69" t="s">
+        <v>130</v>
+      </c>
+      <c r="C69" t="s">
+        <v>150</v>
+      </c>
+      <c r="D69" t="s">
+        <v>132</v>
+      </c>
+      <c r="E69" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>3</v>
+      </c>
+      <c r="B70" t="s">
+        <v>152</v>
+      </c>
+      <c r="C70" t="s">
+        <v>153</v>
+      </c>
+      <c r="D70" t="s">
+        <v>127</v>
+      </c>
+      <c r="E70" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>155</v>
+      </c>
+      <c r="B71" t="s">
+        <v>130</v>
+      </c>
+      <c r="C71" t="s">
+        <v>156</v>
+      </c>
+      <c r="D71" t="s">
+        <v>132</v>
+      </c>
+      <c r="E71" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>3</v>
+      </c>
+      <c r="B72" t="s">
+        <v>152</v>
+      </c>
+      <c r="C72" t="s">
+        <v>158</v>
+      </c>
+      <c r="D72" t="s">
+        <v>127</v>
+      </c>
+      <c r="E72" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>160</v>
+      </c>
+      <c r="B73" t="s">
+        <v>130</v>
+      </c>
+      <c r="C73" t="s">
+        <v>161</v>
+      </c>
+      <c r="D73" t="s">
+        <v>132</v>
+      </c>
+      <c r="E73" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>3</v>
+      </c>
+      <c r="B74" t="s">
+        <v>163</v>
+      </c>
+      <c r="C74" t="s">
+        <v>164</v>
+      </c>
+      <c r="D74" t="s">
+        <v>127</v>
+      </c>
+      <c r="E74" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>166</v>
+      </c>
+      <c r="B75" t="s">
+        <v>130</v>
+      </c>
+      <c r="C75" t="s">
+        <v>167</v>
+      </c>
+      <c r="D75" t="s">
+        <v>132</v>
+      </c>
+      <c r="E75" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>3</v>
+      </c>
+      <c r="B76" t="s">
+        <v>169</v>
+      </c>
+      <c r="C76" t="s">
+        <v>170</v>
+      </c>
+      <c r="D76" t="s">
+        <v>127</v>
+      </c>
+      <c r="E76" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>172</v>
+      </c>
+      <c r="B77" t="s">
+        <v>130</v>
+      </c>
+      <c r="C77" t="s">
+        <v>173</v>
+      </c>
+      <c r="D77" t="s">
+        <v>132</v>
+      </c>
+      <c r="E77" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>3</v>
+      </c>
+      <c r="B78" t="s">
+        <v>3</v>
+      </c>
+      <c r="C78" t="s">
+        <v>175</v>
+      </c>
+      <c r="D78" t="s">
+        <v>176</v>
+      </c>
+      <c r="E78" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>178</v>
+      </c>
+      <c r="B79" t="s">
+        <v>130</v>
+      </c>
+      <c r="C79" t="s">
+        <v>175</v>
+      </c>
+      <c r="D79" t="s">
+        <v>132</v>
+      </c>
+      <c r="E79" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>3</v>
+      </c>
+      <c r="B80" t="s">
+        <v>180</v>
+      </c>
+      <c r="C80" t="s">
+        <v>181</v>
+      </c>
+      <c r="D80" t="s">
+        <v>127</v>
+      </c>
+      <c r="E80" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>183</v>
+      </c>
+      <c r="B81" t="s">
+        <v>130</v>
+      </c>
+      <c r="C81" t="s">
+        <v>184</v>
+      </c>
+      <c r="D81" t="s">
+        <v>132</v>
+      </c>
+      <c r="E81" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>3</v>
+      </c>
+      <c r="B82" t="s">
+        <v>186</v>
+      </c>
+      <c r="C82" t="s">
+        <v>187</v>
+      </c>
+      <c r="D82" t="s">
+        <v>127</v>
+      </c>
+      <c r="E82" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>189</v>
+      </c>
+      <c r="B83" t="s">
+        <v>130</v>
+      </c>
+      <c r="C83" t="s">
+        <v>190</v>
+      </c>
+      <c r="D83" t="s">
+        <v>132</v>
+      </c>
+      <c r="E83" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>3</v>
+      </c>
+      <c r="B84" t="s">
+        <v>192</v>
+      </c>
+      <c r="C84" t="s">
+        <v>193</v>
+      </c>
+      <c r="D84" t="s">
+        <v>127</v>
+      </c>
+      <c r="E84" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>195</v>
+      </c>
+      <c r="B85" t="s">
+        <v>130</v>
+      </c>
+      <c r="C85" t="s">
+        <v>196</v>
+      </c>
+      <c r="D85" t="s">
+        <v>132</v>
+      </c>
+      <c r="E85" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>3</v>
+      </c>
+      <c r="B86" t="s">
+        <v>134</v>
+      </c>
+      <c r="C86" t="s">
+        <v>198</v>
+      </c>
+      <c r="D86" t="s">
+        <v>127</v>
+      </c>
+      <c r="E86" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>200</v>
+      </c>
+      <c r="B87" t="s">
+        <v>130</v>
+      </c>
+      <c r="C87" t="s">
+        <v>201</v>
+      </c>
+      <c r="D87" t="s">
+        <v>132</v>
+      </c>
+      <c r="E87" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>3</v>
+      </c>
+      <c r="B88" t="s">
+        <v>203</v>
+      </c>
+      <c r="C88" t="s">
+        <v>204</v>
+      </c>
+      <c r="D88" t="s">
+        <v>127</v>
+      </c>
+      <c r="E88" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>206</v>
+      </c>
+      <c r="B89" t="s">
+        <v>130</v>
+      </c>
+      <c r="C89" t="s">
+        <v>207</v>
+      </c>
+      <c r="D89" t="s">
+        <v>132</v>
+      </c>
+      <c r="E89" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>3</v>
+      </c>
+      <c r="B90" t="s">
+        <v>209</v>
+      </c>
+      <c r="C90" t="s">
+        <v>210</v>
+      </c>
+      <c r="D90" t="s">
+        <v>127</v>
+      </c>
+      <c r="E90" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>212</v>
+      </c>
+      <c r="B91" t="s">
+        <v>130</v>
+      </c>
+      <c r="C91" t="s">
+        <v>213</v>
+      </c>
+      <c r="D91" t="s">
+        <v>132</v>
+      </c>
+      <c r="E91" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>3</v>
+      </c>
+      <c r="B92" t="s">
+        <v>215</v>
+      </c>
+      <c r="C92" t="s">
+        <v>216</v>
+      </c>
+      <c r="D92" t="s">
+        <v>127</v>
+      </c>
+      <c r="E92" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>218</v>
+      </c>
+      <c r="B93" t="s">
+        <v>130</v>
+      </c>
+      <c r="C93" t="s">
+        <v>219</v>
+      </c>
+      <c r="D93" t="s">
+        <v>132</v>
+      </c>
+      <c r="E93" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>3</v>
+      </c>
+      <c r="B94" t="s">
+        <v>221</v>
+      </c>
+      <c r="C94" t="s">
+        <v>222</v>
+      </c>
+      <c r="D94" t="s">
+        <v>127</v>
+      </c>
+      <c r="E94" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>224</v>
+      </c>
+      <c r="B95" t="s">
+        <v>130</v>
+      </c>
+      <c r="C95" t="s">
+        <v>225</v>
+      </c>
+      <c r="D95" t="s">
+        <v>132</v>
+      </c>
+      <c r="E95" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>3</v>
+      </c>
+      <c r="B96" t="s">
+        <v>227</v>
+      </c>
+      <c r="C96" t="s">
+        <v>228</v>
+      </c>
+      <c r="D96" t="s">
+        <v>127</v>
+      </c>
+      <c r="E96" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>230</v>
+      </c>
+      <c r="B97" t="s">
+        <v>130</v>
+      </c>
+      <c r="C97" t="s">
+        <v>231</v>
+      </c>
+      <c r="D97" t="s">
+        <v>132</v>
+      </c>
+      <c r="E97" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>3</v>
+      </c>
+      <c r="B98" t="s">
+        <v>55</v>
+      </c>
+      <c r="C98" t="s">
+        <v>233</v>
+      </c>
+      <c r="D98" t="s">
+        <v>234</v>
+      </c>
+      <c r="E98" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>236</v>
+      </c>
+      <c r="B99" t="s">
+        <v>130</v>
+      </c>
+      <c r="C99" t="s">
+        <v>233</v>
+      </c>
+      <c r="D99" t="s">
+        <v>132</v>
+      </c>
+      <c r="E99" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>3</v>
+      </c>
+      <c r="B100" t="s">
+        <v>134</v>
+      </c>
+      <c r="C100" t="s">
+        <v>238</v>
+      </c>
+      <c r="D100" t="s">
+        <v>127</v>
+      </c>
+      <c r="E100" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>240</v>
+      </c>
+      <c r="B101" t="s">
+        <v>130</v>
+      </c>
+      <c r="C101" t="s">
+        <v>241</v>
+      </c>
+      <c r="D101" t="s">
+        <v>132</v>
+      </c>
+      <c r="E101" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>3</v>
+      </c>
+      <c r="B102" t="s">
+        <v>243</v>
+      </c>
+      <c r="C102" t="s">
+        <v>244</v>
+      </c>
+      <c r="D102" t="s">
+        <v>127</v>
+      </c>
+      <c r="E102" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>246</v>
+      </c>
+      <c r="B103" t="s">
+        <v>130</v>
+      </c>
+      <c r="C103" t="s">
+        <v>247</v>
+      </c>
+      <c r="D103" t="s">
+        <v>132</v>
+      </c>
+      <c r="E103" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>3</v>
+      </c>
+      <c r="B104" t="s">
+        <v>249</v>
+      </c>
+      <c r="C104" t="s">
+        <v>250</v>
+      </c>
+      <c r="D104" t="s">
+        <v>127</v>
+      </c>
+      <c r="E104" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>252</v>
+      </c>
+      <c r="B105" t="s">
+        <v>130</v>
+      </c>
+      <c r="C105" t="s">
+        <v>253</v>
+      </c>
+      <c r="D105" t="s">
+        <v>132</v>
+      </c>
+      <c r="E105" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>3</v>
+      </c>
+      <c r="B106" t="s">
+        <v>221</v>
+      </c>
+      <c r="C106" t="s">
+        <v>255</v>
+      </c>
+      <c r="D106" t="s">
+        <v>127</v>
+      </c>
+      <c r="E106" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>257</v>
+      </c>
+      <c r="B107" t="s">
+        <v>130</v>
+      </c>
+      <c r="C107" t="s">
+        <v>258</v>
+      </c>
+      <c r="D107" t="s">
+        <v>132</v>
+      </c>
+      <c r="E107" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>3</v>
+      </c>
+      <c r="B108" t="s">
+        <v>260</v>
+      </c>
+      <c r="C108" t="s">
+        <v>261</v>
+      </c>
+      <c r="D108" t="s">
+        <v>127</v>
+      </c>
+      <c r="E108" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>263</v>
+      </c>
+      <c r="B109" t="s">
+        <v>130</v>
+      </c>
+      <c r="C109" t="s">
+        <v>264</v>
+      </c>
+      <c r="D109" t="s">
+        <v>132</v>
+      </c>
+      <c r="E109" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>3</v>
+      </c>
+      <c r="B110" t="s">
+        <v>152</v>
+      </c>
+      <c r="C110" t="s">
+        <v>266</v>
+      </c>
+      <c r="D110" t="s">
+        <v>127</v>
+      </c>
+      <c r="E110" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>268</v>
+      </c>
+      <c r="B111" t="s">
+        <v>130</v>
+      </c>
+      <c r="C111" t="s">
+        <v>269</v>
+      </c>
+      <c r="D111" t="s">
+        <v>132</v>
+      </c>
+      <c r="E111" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>3</v>
+      </c>
+      <c r="B112" t="s">
+        <v>192</v>
+      </c>
+      <c r="C112" t="s">
+        <v>271</v>
+      </c>
+      <c r="D112" t="s">
+        <v>127</v>
+      </c>
+      <c r="E112" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>273</v>
+      </c>
+      <c r="B113" t="s">
+        <v>130</v>
+      </c>
+      <c r="C113" t="s">
+        <v>274</v>
+      </c>
+      <c r="D113" t="s">
+        <v>132</v>
+      </c>
+      <c r="E113" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>3</v>
+      </c>
+      <c r="B114" t="s">
+        <v>221</v>
+      </c>
+      <c r="C114" t="s">
+        <v>276</v>
+      </c>
+      <c r="D114" t="s">
+        <v>127</v>
+      </c>
+      <c r="E114" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>278</v>
+      </c>
+      <c r="B115" t="s">
+        <v>130</v>
+      </c>
+      <c r="C115" t="s">
+        <v>279</v>
+      </c>
+      <c r="D115" t="s">
+        <v>132</v>
+      </c>
+      <c r="E115" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>3</v>
+      </c>
+      <c r="B116" t="s">
+        <v>281</v>
+      </c>
+      <c r="C116" t="s">
+        <v>282</v>
+      </c>
+      <c r="D116" t="s">
+        <v>127</v>
+      </c>
+      <c r="E116" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>284</v>
+      </c>
+      <c r="B117" t="s">
+        <v>130</v>
+      </c>
+      <c r="C117" t="s">
+        <v>285</v>
+      </c>
+      <c r="D117" t="s">
+        <v>132</v>
+      </c>
+      <c r="E117" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>3</v>
+      </c>
+      <c r="B118" t="s">
+        <v>287</v>
+      </c>
+      <c r="C118" t="s">
+        <v>288</v>
+      </c>
+      <c r="D118" t="s">
+        <v>127</v>
+      </c>
+      <c r="E118" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>290</v>
+      </c>
+      <c r="B119" t="s">
+        <v>130</v>
+      </c>
+      <c r="C119" t="s">
+        <v>291</v>
+      </c>
+      <c r="D119" t="s">
+        <v>132</v>
+      </c>
+      <c r="E119" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>3</v>
+      </c>
+      <c r="B120" t="s">
+        <v>249</v>
+      </c>
+      <c r="C120" t="s">
+        <v>293</v>
+      </c>
+      <c r="D120" t="s">
+        <v>127</v>
+      </c>
+      <c r="E120" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>295</v>
+      </c>
+      <c r="B121" t="s">
+        <v>130</v>
+      </c>
+      <c r="C121" t="s">
+        <v>296</v>
+      </c>
+      <c r="D121" t="s">
+        <v>132</v>
+      </c>
+      <c r="E121" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>3</v>
+      </c>
+      <c r="B122" t="s">
+        <v>203</v>
+      </c>
+      <c r="C122" t="s">
+        <v>298</v>
+      </c>
+      <c r="D122" t="s">
+        <v>127</v>
+      </c>
+      <c r="E122" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>300</v>
+      </c>
+      <c r="B123" t="s">
+        <v>130</v>
+      </c>
+      <c r="C123" t="s">
+        <v>301</v>
+      </c>
+      <c r="D123" t="s">
+        <v>132</v>
+      </c>
+      <c r="E123" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>3</v>
+      </c>
+      <c r="B124" t="s">
+        <v>303</v>
+      </c>
+      <c r="C124" t="s">
+        <v>304</v>
+      </c>
+      <c r="D124" t="s">
+        <v>127</v>
+      </c>
+      <c r="E124" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>306</v>
+      </c>
+      <c r="B125" t="s">
+        <v>130</v>
+      </c>
+      <c r="C125" t="s">
+        <v>307</v>
+      </c>
+      <c r="D125" t="s">
+        <v>132</v>
+      </c>
+      <c r="E125" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>3</v>
+      </c>
+      <c r="B126" t="s">
+        <v>309</v>
+      </c>
+      <c r="C126" t="s">
+        <v>310</v>
+      </c>
+      <c r="D126" t="s">
+        <v>127</v>
+      </c>
+      <c r="E126" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>312</v>
+      </c>
+      <c r="B127" t="s">
+        <v>130</v>
+      </c>
+      <c r="C127" t="s">
+        <v>313</v>
+      </c>
+      <c r="D127" t="s">
+        <v>132</v>
+      </c>
+      <c r="E127" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>3</v>
+      </c>
+      <c r="B128" t="s">
+        <v>163</v>
+      </c>
+      <c r="C128" t="s">
+        <v>315</v>
+      </c>
+      <c r="D128" t="s">
+        <v>127</v>
+      </c>
+      <c r="E128" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>317</v>
+      </c>
+      <c r="B129" t="s">
+        <v>130</v>
+      </c>
+      <c r="C129" t="s">
+        <v>318</v>
+      </c>
+      <c r="D129" t="s">
+        <v>132</v>
+      </c>
+      <c r="E129" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>3</v>
+      </c>
+      <c r="B130" t="s">
+        <v>203</v>
+      </c>
+      <c r="C130" t="s">
+        <v>320</v>
+      </c>
+      <c r="D130" t="s">
+        <v>127</v>
+      </c>
+      <c r="E130" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>322</v>
+      </c>
+      <c r="B131" t="s">
+        <v>130</v>
+      </c>
+      <c r="C131" t="s">
+        <v>323</v>
+      </c>
+      <c r="D131" t="s">
+        <v>132</v>
+      </c>
+      <c r="E131" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>3</v>
+      </c>
+      <c r="B132" t="s">
+        <v>227</v>
+      </c>
+      <c r="C132" t="s">
+        <v>325</v>
+      </c>
+      <c r="D132" t="s">
+        <v>127</v>
+      </c>
+      <c r="E132" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>327</v>
+      </c>
+      <c r="B133" t="s">
+        <v>130</v>
+      </c>
+      <c r="C133" t="s">
+        <v>328</v>
+      </c>
+      <c r="D133" t="s">
+        <v>132</v>
+      </c>
+      <c r="E133" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>3</v>
+      </c>
+      <c r="B134" t="s">
+        <v>221</v>
+      </c>
+      <c r="C134" t="s">
+        <v>330</v>
+      </c>
+      <c r="D134" t="s">
+        <v>127</v>
+      </c>
+      <c r="E134" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>332</v>
+      </c>
+      <c r="B135" t="s">
+        <v>130</v>
+      </c>
+      <c r="C135" t="s">
+        <v>333</v>
+      </c>
+      <c r="D135" t="s">
+        <v>132</v>
+      </c>
+      <c r="E135" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>3</v>
+      </c>
+      <c r="B136" t="s">
+        <v>152</v>
+      </c>
+      <c r="C136" t="s">
+        <v>335</v>
+      </c>
+      <c r="D136" t="s">
+        <v>127</v>
+      </c>
+      <c r="E136" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>337</v>
+      </c>
+      <c r="B137" t="s">
+        <v>130</v>
+      </c>
+      <c r="C137" t="s">
+        <v>338</v>
+      </c>
+      <c r="D137" t="s">
+        <v>132</v>
+      </c>
+      <c r="E137" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>3</v>
+      </c>
+      <c r="B138" t="s">
+        <v>192</v>
+      </c>
+      <c r="C138" t="s">
+        <v>340</v>
+      </c>
+      <c r="D138" t="s">
+        <v>127</v>
+      </c>
+      <c r="E138" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>342</v>
+      </c>
+      <c r="B139" t="s">
+        <v>130</v>
+      </c>
+      <c r="C139" t="s">
+        <v>343</v>
+      </c>
+      <c r="D139" t="s">
+        <v>132</v>
+      </c>
+      <c r="E139" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>3</v>
+      </c>
+      <c r="B140" t="s">
+        <v>345</v>
+      </c>
+      <c r="C140" t="s">
+        <v>346</v>
+      </c>
+      <c r="D140" t="s">
+        <v>127</v>
+      </c>
+      <c r="E140" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>348</v>
+      </c>
+      <c r="B141" t="s">
+        <v>130</v>
+      </c>
+      <c r="C141" t="s">
+        <v>349</v>
+      </c>
+      <c r="D141" t="s">
+        <v>132</v>
+      </c>
+      <c r="E141" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>3</v>
+      </c>
+      <c r="B142" t="s">
+        <v>227</v>
+      </c>
+      <c r="C142" t="s">
+        <v>351</v>
+      </c>
+      <c r="D142" t="s">
+        <v>127</v>
+      </c>
+      <c r="E142" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>353</v>
+      </c>
+      <c r="B143" t="s">
+        <v>130</v>
+      </c>
+      <c r="C143" t="s">
+        <v>354</v>
+      </c>
+      <c r="D143" t="s">
+        <v>132</v>
+      </c>
+      <c r="E143" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>3</v>
+      </c>
+      <c r="B144" t="s">
+        <v>356</v>
+      </c>
+      <c r="C144" t="s">
+        <v>357</v>
+      </c>
+      <c r="D144" t="s">
+        <v>127</v>
+      </c>
+      <c r="E144" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>359</v>
+      </c>
+      <c r="B145" t="s">
+        <v>130</v>
+      </c>
+      <c r="C145" t="s">
+        <v>360</v>
+      </c>
+      <c r="D145" t="s">
+        <v>132</v>
+      </c>
+      <c r="E145" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>3</v>
+      </c>
+      <c r="B146" t="s">
+        <v>192</v>
+      </c>
+      <c r="C146" t="s">
+        <v>362</v>
+      </c>
+      <c r="D146" t="s">
+        <v>127</v>
+      </c>
+      <c r="E146" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>364</v>
+      </c>
+      <c r="B147" t="s">
+        <v>130</v>
+      </c>
+      <c r="C147" t="s">
+        <v>365</v>
+      </c>
+      <c r="D147" t="s">
+        <v>132</v>
+      </c>
+      <c r="E147" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>3</v>
+      </c>
+      <c r="B148" t="s">
+        <v>356</v>
+      </c>
+      <c r="C148" t="s">
+        <v>367</v>
+      </c>
+      <c r="D148" t="s">
+        <v>127</v>
+      </c>
+      <c r="E148" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>369</v>
+      </c>
+      <c r="B149" t="s">
+        <v>130</v>
+      </c>
+      <c r="C149" t="s">
+        <v>370</v>
+      </c>
+      <c r="D149" t="s">
+        <v>132</v>
+      </c>
+      <c r="E149" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>3</v>
+      </c>
+      <c r="B150" t="s">
+        <v>243</v>
+      </c>
+      <c r="C150" t="s">
+        <v>372</v>
+      </c>
+      <c r="D150" t="s">
+        <v>127</v>
+      </c>
+      <c r="E150" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>374</v>
+      </c>
+      <c r="B151" t="s">
+        <v>130</v>
+      </c>
+      <c r="C151" t="s">
+        <v>375</v>
+      </c>
+      <c r="D151" t="s">
+        <v>132</v>
+      </c>
+      <c r="E151" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>3</v>
+      </c>
+      <c r="B152" t="s">
+        <v>140</v>
+      </c>
+      <c r="C152" t="s">
+        <v>377</v>
+      </c>
+      <c r="D152" t="s">
+        <v>127</v>
+      </c>
+      <c r="E152" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>379</v>
+      </c>
+      <c r="B153" t="s">
+        <v>130</v>
+      </c>
+      <c r="C153" t="s">
+        <v>380</v>
+      </c>
+      <c r="D153" t="s">
+        <v>132</v>
+      </c>
+      <c r="E153" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>3</v>
+      </c>
+      <c r="B154" t="s">
+        <v>356</v>
+      </c>
+      <c r="C154" t="s">
+        <v>382</v>
+      </c>
+      <c r="D154" t="s">
+        <v>127</v>
+      </c>
+      <c r="E154" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>384</v>
+      </c>
+      <c r="B155" t="s">
+        <v>130</v>
+      </c>
+      <c r="C155" t="s">
+        <v>385</v>
+      </c>
+      <c r="D155" t="s">
+        <v>132</v>
+      </c>
+      <c r="E155" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>3</v>
+      </c>
+      <c r="B156" t="s">
+        <v>140</v>
+      </c>
+      <c r="C156" t="s">
+        <v>387</v>
+      </c>
+      <c r="D156" t="s">
+        <v>127</v>
+      </c>
+      <c r="E156" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>389</v>
+      </c>
+      <c r="B157" t="s">
+        <v>130</v>
+      </c>
+      <c r="C157" t="s">
+        <v>390</v>
+      </c>
+      <c r="D157" t="s">
+        <v>132</v>
+      </c>
+      <c r="E157" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
+        <v>3</v>
+      </c>
+      <c r="B158" t="s">
+        <v>152</v>
+      </c>
+      <c r="C158" t="s">
+        <v>392</v>
+      </c>
+      <c r="D158" t="s">
+        <v>127</v>
+      </c>
+      <c r="E158" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>394</v>
+      </c>
+      <c r="B159" t="s">
+        <v>130</v>
+      </c>
+      <c r="C159" t="s">
+        <v>395</v>
+      </c>
+      <c r="D159" t="s">
+        <v>132</v>
+      </c>
+      <c r="E159" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>3</v>
+      </c>
+      <c r="B160" t="s">
+        <v>397</v>
+      </c>
+      <c r="C160" t="s">
+        <v>398</v>
+      </c>
+      <c r="D160" t="s">
+        <v>127</v>
+      </c>
+      <c r="E160" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>400</v>
+      </c>
+      <c r="B161" t="s">
+        <v>130</v>
+      </c>
+      <c r="C161" t="s">
+        <v>401</v>
+      </c>
+      <c r="D161" t="s">
+        <v>132</v>
+      </c>
+      <c r="E161" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>3</v>
+      </c>
+      <c r="B162" t="s">
+        <v>203</v>
+      </c>
+      <c r="C162" t="s">
+        <v>403</v>
+      </c>
+      <c r="D162" t="s">
+        <v>127</v>
+      </c>
+      <c r="E162" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>405</v>
+      </c>
+      <c r="B163" t="s">
+        <v>130</v>
+      </c>
+      <c r="C163" t="s">
+        <v>406</v>
+      </c>
+      <c r="D163" t="s">
+        <v>132</v>
+      </c>
+      <c r="E163" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>3</v>
+      </c>
+      <c r="B164" t="s">
+        <v>140</v>
+      </c>
+      <c r="C164" t="s">
+        <v>408</v>
+      </c>
+      <c r="D164" t="s">
+        <v>127</v>
+      </c>
+      <c r="E164" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>410</v>
+      </c>
+      <c r="B165" t="s">
+        <v>130</v>
+      </c>
+      <c r="C165" t="s">
+        <v>411</v>
+      </c>
+      <c r="D165" t="s">
+        <v>132</v>
+      </c>
+      <c r="E165" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>3</v>
+      </c>
+      <c r="B166" t="s">
+        <v>186</v>
+      </c>
+      <c r="C166" t="s">
+        <v>413</v>
+      </c>
+      <c r="D166" t="s">
+        <v>127</v>
+      </c>
+      <c r="E166" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>415</v>
+      </c>
+      <c r="B167" t="s">
+        <v>130</v>
+      </c>
+      <c r="C167" t="s">
+        <v>416</v>
+      </c>
+      <c r="D167" t="s">
+        <v>132</v>
+      </c>
+      <c r="E167" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>3</v>
+      </c>
+      <c r="B168" t="s">
+        <v>281</v>
+      </c>
+      <c r="C168" t="s">
+        <v>418</v>
+      </c>
+      <c r="D168" t="s">
+        <v>127</v>
+      </c>
+      <c r="E168" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>420</v>
+      </c>
+      <c r="B169" t="s">
+        <v>130</v>
+      </c>
+      <c r="C169" t="s">
+        <v>421</v>
+      </c>
+      <c r="D169" t="s">
+        <v>132</v>
+      </c>
+      <c r="E169" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>3</v>
+      </c>
+      <c r="B170" t="s">
+        <v>163</v>
+      </c>
+      <c r="C170" t="s">
+        <v>423</v>
+      </c>
+      <c r="D170" t="s">
+        <v>127</v>
+      </c>
+      <c r="E170" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>425</v>
+      </c>
+      <c r="B171" t="s">
+        <v>130</v>
+      </c>
+      <c r="C171" t="s">
+        <v>426</v>
+      </c>
+      <c r="D171" t="s">
+        <v>132</v>
+      </c>
+      <c r="E171" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>3</v>
+      </c>
+      <c r="B172" t="s">
+        <v>203</v>
+      </c>
+      <c r="C172" t="s">
+        <v>428</v>
+      </c>
+      <c r="D172" t="s">
+        <v>127</v>
+      </c>
+      <c r="E172" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>430</v>
+      </c>
+      <c r="B173" t="s">
+        <v>130</v>
+      </c>
+      <c r="C173" t="s">
+        <v>431</v>
+      </c>
+      <c r="D173" t="s">
+        <v>132</v>
+      </c>
+      <c r="E173" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>3</v>
+      </c>
+      <c r="B174" t="s">
+        <v>309</v>
+      </c>
+      <c r="C174" t="s">
+        <v>433</v>
+      </c>
+      <c r="D174" t="s">
+        <v>127</v>
+      </c>
+      <c r="E174" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
+        <v>435</v>
+      </c>
+      <c r="B175" t="s">
+        <v>130</v>
+      </c>
+      <c r="C175" t="s">
+        <v>436</v>
+      </c>
+      <c r="D175" t="s">
+        <v>132</v>
+      </c>
+      <c r="E175" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>3</v>
+      </c>
+      <c r="B176" t="s">
+        <v>134</v>
+      </c>
+      <c r="C176" t="s">
+        <v>438</v>
+      </c>
+      <c r="D176" t="s">
+        <v>127</v>
+      </c>
+      <c r="E176" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>440</v>
+      </c>
+      <c r="B177" t="s">
+        <v>130</v>
+      </c>
+      <c r="C177" t="s">
+        <v>441</v>
+      </c>
+      <c r="D177" t="s">
+        <v>132</v>
+      </c>
+      <c r="E177" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>3</v>
+      </c>
+      <c r="B178" t="s">
+        <v>125</v>
+      </c>
+      <c r="C178" t="s">
+        <v>443</v>
+      </c>
+      <c r="D178" t="s">
+        <v>127</v>
+      </c>
+      <c r="E178" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>445</v>
+      </c>
+      <c r="B179" t="s">
+        <v>130</v>
+      </c>
+      <c r="C179" t="s">
+        <v>446</v>
+      </c>
+      <c r="D179" t="s">
+        <v>132</v>
+      </c>
+      <c r="E179" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>3</v>
+      </c>
+      <c r="B180" t="s">
+        <v>303</v>
+      </c>
+      <c r="C180" t="s">
+        <v>448</v>
+      </c>
+      <c r="D180" t="s">
+        <v>127</v>
+      </c>
+      <c r="E180" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
+        <v>450</v>
+      </c>
+      <c r="B181" t="s">
+        <v>130</v>
+      </c>
+      <c r="C181" t="s">
+        <v>451</v>
+      </c>
+      <c r="D181" t="s">
+        <v>132</v>
+      </c>
+      <c r="E181" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A182" t="s">
+        <v>3</v>
+      </c>
+      <c r="B182" t="s">
+        <v>140</v>
+      </c>
+      <c r="C182" t="s">
+        <v>453</v>
+      </c>
+      <c r="D182" t="s">
+        <v>127</v>
+      </c>
+      <c r="E182" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
+        <v>455</v>
+      </c>
+      <c r="B183" t="s">
+        <v>130</v>
+      </c>
+      <c r="C183" t="s">
+        <v>456</v>
+      </c>
+      <c r="D183" t="s">
+        <v>132</v>
+      </c>
+      <c r="E183" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
+        <v>3</v>
+      </c>
+      <c r="B184" t="s">
+        <v>227</v>
+      </c>
+      <c r="C184" t="s">
+        <v>458</v>
+      </c>
+      <c r="D184" t="s">
+        <v>127</v>
+      </c>
+      <c r="E184" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
+        <v>460</v>
+      </c>
+      <c r="B185" t="s">
+        <v>130</v>
+      </c>
+      <c r="C185" t="s">
+        <v>461</v>
+      </c>
+      <c r="D185" t="s">
+        <v>132</v>
+      </c>
+      <c r="E185" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
+        <v>3</v>
+      </c>
+      <c r="B186" t="s">
+        <v>463</v>
+      </c>
+      <c r="C186" t="s">
+        <v>464</v>
+      </c>
+      <c r="D186" t="s">
+        <v>127</v>
+      </c>
+      <c r="E186" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
+        <v>466</v>
+      </c>
+      <c r="B187" t="s">
+        <v>130</v>
+      </c>
+      <c r="C187" t="s">
+        <v>467</v>
+      </c>
+      <c r="D187" t="s">
+        <v>132</v>
+      </c>
+      <c r="E187" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A188" t="s">
+        <v>3</v>
+      </c>
+      <c r="B188" t="s">
+        <v>469</v>
+      </c>
+      <c r="C188" t="s">
+        <v>470</v>
+      </c>
+      <c r="D188" t="s">
+        <v>127</v>
+      </c>
+      <c r="E188" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A189" t="s">
+        <v>472</v>
+      </c>
+      <c r="B189" t="s">
+        <v>130</v>
+      </c>
+      <c r="C189" t="s">
+        <v>473</v>
+      </c>
+      <c r="D189" t="s">
+        <v>132</v>
+      </c>
+      <c r="E189" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A190" t="s">
+        <v>3</v>
+      </c>
+      <c r="B190" t="s">
+        <v>249</v>
+      </c>
+      <c r="C190" t="s">
+        <v>475</v>
+      </c>
+      <c r="D190" t="s">
+        <v>127</v>
+      </c>
+      <c r="E190" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
+        <v>477</v>
+      </c>
+      <c r="B191" t="s">
+        <v>130</v>
+      </c>
+      <c r="C191" t="s">
+        <v>478</v>
+      </c>
+      <c r="D191" t="s">
+        <v>132</v>
+      </c>
+      <c r="E191" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A192" t="s">
+        <v>3</v>
+      </c>
+      <c r="B192" t="s">
+        <v>345</v>
+      </c>
+      <c r="C192" t="s">
+        <v>480</v>
+      </c>
+      <c r="D192" t="s">
+        <v>127</v>
+      </c>
+      <c r="E192" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
+        <v>482</v>
+      </c>
+      <c r="B193" t="s">
+        <v>130</v>
+      </c>
+      <c r="C193" t="s">
+        <v>483</v>
+      </c>
+      <c r="D193" t="s">
+        <v>132</v>
+      </c>
+      <c r="E193" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
+        <v>3</v>
+      </c>
+      <c r="B194" t="s">
+        <v>169</v>
+      </c>
+      <c r="C194" t="s">
+        <v>485</v>
+      </c>
+      <c r="D194" t="s">
+        <v>127</v>
+      </c>
+      <c r="E194" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A195" t="s">
+        <v>487</v>
+      </c>
+      <c r="B195" t="s">
+        <v>130</v>
+      </c>
+      <c r="C195" t="s">
+        <v>488</v>
+      </c>
+      <c r="D195" t="s">
+        <v>132</v>
+      </c>
+      <c r="E195" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
+        <v>3</v>
+      </c>
+      <c r="B196" t="s">
+        <v>134</v>
+      </c>
+      <c r="C196" t="s">
+        <v>490</v>
+      </c>
+      <c r="D196" t="s">
+        <v>127</v>
+      </c>
+      <c r="E196" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A197" t="s">
+        <v>492</v>
+      </c>
+      <c r="B197" t="s">
+        <v>130</v>
+      </c>
+      <c r="C197" t="s">
+        <v>493</v>
+      </c>
+      <c r="D197" t="s">
+        <v>132</v>
+      </c>
+      <c r="E197" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A198" t="s">
+        <v>3</v>
+      </c>
+      <c r="B198" t="s">
+        <v>192</v>
+      </c>
+      <c r="C198" t="s">
+        <v>495</v>
+      </c>
+      <c r="D198" t="s">
+        <v>127</v>
+      </c>
+      <c r="E198" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A199" t="s">
+        <v>497</v>
+      </c>
+      <c r="B199" t="s">
+        <v>130</v>
+      </c>
+      <c r="C199" t="s">
+        <v>498</v>
+      </c>
+      <c r="D199" t="s">
+        <v>132</v>
+      </c>
+      <c r="E199" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
+        <v>3</v>
+      </c>
+      <c r="B200" t="s">
+        <v>249</v>
+      </c>
+      <c r="C200" t="s">
+        <v>500</v>
+      </c>
+      <c r="D200" t="s">
+        <v>127</v>
+      </c>
+      <c r="E200" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A201" t="s">
+        <v>502</v>
+      </c>
+      <c r="B201" t="s">
+        <v>130</v>
+      </c>
+      <c r="C201" t="s">
+        <v>503</v>
+      </c>
+      <c r="D201" t="s">
+        <v>132</v>
+      </c>
+      <c r="E201" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
+        <v>3</v>
+      </c>
+      <c r="B202" t="s">
+        <v>249</v>
+      </c>
+      <c r="C202" t="s">
+        <v>505</v>
+      </c>
+      <c r="D202" t="s">
+        <v>127</v>
+      </c>
+      <c r="E202" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A203" t="s">
+        <v>507</v>
+      </c>
+      <c r="B203" t="s">
+        <v>130</v>
+      </c>
+      <c r="C203" t="s">
+        <v>508</v>
+      </c>
+      <c r="D203" t="s">
+        <v>132</v>
+      </c>
+      <c r="E203" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A204" t="s">
+        <v>3</v>
+      </c>
+      <c r="B204" t="s">
+        <v>309</v>
+      </c>
+      <c r="C204" t="s">
+        <v>510</v>
+      </c>
+      <c r="D204" t="s">
+        <v>127</v>
+      </c>
+      <c r="E204" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A205" t="s">
+        <v>512</v>
+      </c>
+      <c r="B205" t="s">
+        <v>130</v>
+      </c>
+      <c r="C205" t="s">
+        <v>513</v>
+      </c>
+      <c r="D205" t="s">
+        <v>132</v>
+      </c>
+      <c r="E205" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A206" t="s">
+        <v>3</v>
+      </c>
+      <c r="B206" t="s">
+        <v>249</v>
+      </c>
+      <c r="C206" t="s">
+        <v>515</v>
+      </c>
+      <c r="D206" t="s">
+        <v>127</v>
+      </c>
+      <c r="E206" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A207" t="s">
+        <v>517</v>
+      </c>
+      <c r="B207" t="s">
+        <v>130</v>
+      </c>
+      <c r="C207" t="s">
+        <v>518</v>
+      </c>
+      <c r="D207" t="s">
+        <v>132</v>
+      </c>
+      <c r="E207" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A208" t="s">
+        <v>3</v>
+      </c>
+      <c r="B208" t="s">
+        <v>221</v>
+      </c>
+      <c r="C208" t="s">
+        <v>520</v>
+      </c>
+      <c r="D208" t="s">
+        <v>127</v>
+      </c>
+      <c r="E208" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A209" t="s">
+        <v>522</v>
+      </c>
+      <c r="B209" t="s">
+        <v>130</v>
+      </c>
+      <c r="C209" t="s">
+        <v>523</v>
+      </c>
+      <c r="D209" t="s">
+        <v>132</v>
+      </c>
+      <c r="E209" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A210" t="s">
+        <v>3</v>
+      </c>
+      <c r="B210" t="s">
+        <v>203</v>
+      </c>
+      <c r="C210" t="s">
+        <v>525</v>
+      </c>
+      <c r="D210" t="s">
+        <v>127</v>
+      </c>
+      <c r="E210" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
+        <v>527</v>
+      </c>
+      <c r="B211" t="s">
+        <v>130</v>
+      </c>
+      <c r="C211" t="s">
+        <v>528</v>
+      </c>
+      <c r="D211" t="s">
+        <v>132</v>
+      </c>
+      <c r="E211" t="s">
+        <v>529</v>
       </c>
     </row>
   </sheetData>
@@ -1642,44 +5406,44 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
fiz a tipagem do módulo achievement
</commit_message>
<xml_diff>
--- a/data/csv/Fusao.xlsx
+++ b/data/csv/Fusao.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elisa\Desktop\FGV\LP\elemental_fusion_game\data\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{505A67B2-0441-4935-8990-1F6A9561084E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2337B7C-41A6-4124-9652-FFCBB2438FEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0EEE3841-29D7-4E79-BA1B-2D13D8D18CD6}"/>
   </bookViews>
@@ -2147,7 +2147,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1D720B-7551-40E6-A447-F5FBB3C0D518}">
   <dimension ref="A1:E211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -2156,7 +2156,7 @@
     <col min="1" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="105.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="116.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
adicionei algumas fusões e uma lista com os elementos faltantes em game
</commit_message>
<xml_diff>
--- a/data/csv/Fusao.xlsx
+++ b/data/csv/Fusao.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raphy\elemental_fusion_game\data\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83D4EB6-83F3-42A5-B237-4D51841C38BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB66C01-7D80-483F-9AE6-F734FE7721FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0EEE3841-29D7-4E79-BA1B-2D13D8D18CD6}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{0EEE3841-29D7-4E79-BA1B-2D13D8D18CD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="205">
   <si>
     <t>H-1</t>
   </si>
@@ -553,6 +553,105 @@
   </si>
   <si>
     <t>O Oxigênio-18 é um isótopo estável do oxigênio utilizado em estudos isotópicos.</t>
+  </si>
+  <si>
+    <t>K-39, n</t>
+  </si>
+  <si>
+    <t>Ar-38</t>
+  </si>
+  <si>
+    <t>K-39, y</t>
+  </si>
+  <si>
+    <t>K-39</t>
+  </si>
+  <si>
+    <t>K-40</t>
+  </si>
+  <si>
+    <t>K-41</t>
+  </si>
+  <si>
+    <t>Cr-50</t>
+  </si>
+  <si>
+    <t>Mn-51</t>
+  </si>
+  <si>
+    <t>Mn-51, y</t>
+  </si>
+  <si>
+    <t>Fe-51</t>
+  </si>
+  <si>
+    <t>Fe-51, e+, ve</t>
+  </si>
+  <si>
+    <t>Co-52, y</t>
+  </si>
+  <si>
+    <t>Co-52</t>
+  </si>
+  <si>
+    <t>V-51, e+, ve</t>
+  </si>
+  <si>
+    <t>Ti-49</t>
+  </si>
+  <si>
+    <t>Ti-50</t>
+  </si>
+  <si>
+    <t>V-51, y</t>
+  </si>
+  <si>
+    <t>V-51</t>
+  </si>
+  <si>
+    <t>V-52</t>
+  </si>
+  <si>
+    <t>Cr-52, e+, ve</t>
+  </si>
+  <si>
+    <t>V-50, ve</t>
+  </si>
+  <si>
+    <t>Cr-54</t>
+  </si>
+  <si>
+    <t>Mn-55, y</t>
+  </si>
+  <si>
+    <t>O cromo-54 captura um próton, resultando em manganês-55.</t>
+  </si>
+  <si>
+    <t>Mn-54</t>
+  </si>
+  <si>
+    <t>Mn-55</t>
+  </si>
+  <si>
+    <t>O manganês-54 captura um nêutron para formar manganês-55.</t>
+  </si>
+  <si>
+    <t>O vanádio-50 pode ser formado a partir do vanádio-51 através de captura eletrônica durante processos de captura lenta de nêutrons.</t>
+  </si>
+  <si>
+    <t>Através de uma série de capturas de prótons e decaimentos beta, cromo-50 pode eventualmente levar à formação de vanádio-51</t>
+  </si>
+  <si>
+    <t>O potássio-40 captura outro nêutron, resultando em potássio-41</t>
+  </si>
+  <si>
+    <t>O potássio-39 pode capturar um nêutron livre durante processos de captura lenta de nêutrons (s-process), formando potássio-40.</t>
+  </si>
+  <si>
+    <t>O argônio-38 pode capturar um próton para formar potássio-39, emitindo um raio gama.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O argônio-36 pode capturar uma partícula alfa, resultando na formação de potássio-39 e liberando um nêutron.</t>
   </si>
 </sst>
 </file>
@@ -930,10 +1029,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1D720B-7551-40E6-A447-F5FBB3C0D518}">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E62" sqref="A62:E211"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1910,6 +2009,186 @@
       </c>
       <c r="E61" t="s">
         <v>171</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>33</v>
+      </c>
+      <c r="B62" t="s">
+        <v>3</v>
+      </c>
+      <c r="C62" t="s">
+        <v>172</v>
+      </c>
+      <c r="E62" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>173</v>
+      </c>
+      <c r="B63" t="s">
+        <v>0</v>
+      </c>
+      <c r="C63" t="s">
+        <v>174</v>
+      </c>
+      <c r="E63" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>175</v>
+      </c>
+      <c r="B64" t="s">
+        <v>15</v>
+      </c>
+      <c r="C64" t="s">
+        <v>176</v>
+      </c>
+      <c r="E64" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>176</v>
+      </c>
+      <c r="B65" t="s">
+        <v>15</v>
+      </c>
+      <c r="C65" t="s">
+        <v>177</v>
+      </c>
+      <c r="E65" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>178</v>
+      </c>
+      <c r="B66" t="s">
+        <v>0</v>
+      </c>
+      <c r="C66" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>179</v>
+      </c>
+      <c r="C67" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>181</v>
+      </c>
+      <c r="B68" t="s">
+        <v>0</v>
+      </c>
+      <c r="C68" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>184</v>
+      </c>
+      <c r="C69" t="s">
+        <v>185</v>
+      </c>
+      <c r="E69" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>186</v>
+      </c>
+      <c r="B70" t="s">
+        <v>15</v>
+      </c>
+      <c r="C70" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>187</v>
+      </c>
+      <c r="B71" t="s">
+        <v>0</v>
+      </c>
+      <c r="C71" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>189</v>
+      </c>
+      <c r="B72" t="s">
+        <v>15</v>
+      </c>
+      <c r="C72" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>190</v>
+      </c>
+      <c r="C73" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>189</v>
+      </c>
+      <c r="B74" t="s">
+        <v>12</v>
+      </c>
+      <c r="C74" t="s">
+        <v>192</v>
+      </c>
+      <c r="E74" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>193</v>
+      </c>
+      <c r="B75" t="s">
+        <v>0</v>
+      </c>
+      <c r="C75" t="s">
+        <v>194</v>
+      </c>
+      <c r="E75" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>196</v>
+      </c>
+      <c r="B76" t="s">
+        <v>15</v>
+      </c>
+      <c r="C76" t="s">
+        <v>197</v>
+      </c>
+      <c r="E76" t="s">
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>